<commit_message>
Ajout data file + variables
</commit_message>
<xml_diff>
--- a/dolibarr_auto/Data Files/VariablesTiers.xlsx
+++ b/dolibarr_auto/Data Files/VariablesTiers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\gitProjects2\Automatisation_dolibarr\dolibarr_auto\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB046D66-CE1D-4EDA-8282-17DF809D0B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C5A040-BC96-4BC0-B0EA-70D54E6CE0EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13455" yWindow="5505" windowWidth="16140" windowHeight="12045"/>
+    <workbookView xWindow="13455" yWindow="5505" windowWidth="16140" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>NomEntreprise</t>
-  </si>
-  <si>
     <t>April</t>
   </si>
   <si>
-    <t>Prospect/Client</t>
+    <t>Client</t>
   </si>
   <si>
-    <t>Client</t>
+    <t>nomTiers</t>
+  </si>
+  <si>
+    <t>clientProspect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -396,32 +396,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>